<commit_message>
Update tick stream in Excel
</commit_message>
<xml_diff>
--- a/src/adaptors/xll/sheets/MarketData.xlsx
+++ b/src/adaptors/xll/sheets/MarketData.xlsx
@@ -1,31 +1,61 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\trading\crypto\src\adaptors\xll\sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\trading\crypto\src\adaptors\xll\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976833E1-F274-48BB-A311-5F7F57EC1B87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E3232B-36E4-4A57-9D1C-959AD36449F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27840" yWindow="10335" windowWidth="27345" windowHeight="17970" xr2:uid="{6EC07C23-A19E-4BD9-8DD5-112772866BDB}"/>
+    <workbookView xWindow="14895" yWindow="14715" windowWidth="28770" windowHeight="15570" xr2:uid="{6EC07C23-A19E-4BD9-8DD5-112772866BDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>subscribe</t>
   </si>
@@ -33,9 +63,6 @@
     <t>SecCode</t>
   </si>
   <si>
-    <t>OK</t>
-  </si>
-  <si>
     <t>BTC/USD</t>
   </si>
   <si>
@@ -69,18 +96,26 @@
     <t>time</t>
   </si>
   <si>
-    <t>Invalid request</t>
-  </si>
-  <si>
     <t>DUMMY</t>
+  </si>
+  <si>
+    <t>ADABULL/USD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -108,8 +143,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,16 +460,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA93EA7B-8889-4B84-AA0B-ACE2D2DC5BF2}">
-  <dimension ref="B2:F16"/>
+  <dimension ref="B2:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
@@ -441,71 +477,80 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>2</v>
+      <c r="B3" t="str" cm="1">
+        <f t="array" ref="B3">_xll.SUBSCRIBE(C3)</f>
+        <v>OK</v>
       </c>
       <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="str" cm="1">
+        <f t="array" ref="B4">_xll.SUBSCRIBE(C4)</f>
+        <v>OK</v>
+      </c>
+      <c r="C4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="str" cm="1">
+        <f t="array" ref="B5">_xll.SUBSCRIBE(C5)</f>
+        <v>OK</v>
+      </c>
+      <c r="C5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
       </c>
       <c r="D7" t="s">
         <v>1</v>
       </c>
       <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" cm="1">
+        <f t="array" ref="B8">_xll.TICK(C8,D8)</f>
+        <v>2249</v>
+      </c>
+      <c r="D8" t="str">
+        <f>$C$3</f>
+        <v>ADABULL/USD</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" cm="1">
+        <f t="array" ref="B9">_xll.TICK(C9,D9)</f>
+        <v>2249</v>
+      </c>
+      <c r="C9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>36282.5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>36282.5</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D9" t="str">
+        <f t="shared" ref="D9:D13" si="0">$C$3</f>
+        <v>ADABULL/USD</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" cm="1">
+        <f t="array" ref="B10">_xll.TICK(C10,D10)</f>
+        <v>2238</v>
+      </c>
+      <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="D9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>36278</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>3</v>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>ADABULL/USD</v>
       </c>
       <c r="E10">
         <v>36282.5</v>
@@ -515,72 +560,91 @@
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>36287</v>
+      <c r="B11" cm="1">
+        <f t="array" ref="B11">_xll.TICK(C11,D11)</f>
+        <v>2260</v>
       </c>
       <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>ADABULL/USD</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" cm="1">
+        <f t="array" ref="B12">_xll.TICK(C12,D12)</f>
+        <v>2239</v>
+      </c>
+      <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>ADABULL/USD</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" cm="1">
+        <f t="array" ref="B13">_xll.TICK(C13,D13)</f>
+        <v>1623128839.982069</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>ADABULL/USD</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" cm="1">
+        <f t="array" ref="B14">_xll.TICK(C14,D14)</f>
+        <v>32937.5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" cm="1">
+        <f t="array" ref="B15">_xll.TICK(C15,D15)</f>
+        <v>2505.5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>36287</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>1623044461</v>
-      </c>
-      <c r="C13" t="s">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" cm="1">
+        <f t="array" ref="B16">_xll.TICK(C16,D16)</f>
+        <v>0.85882499999999995</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="str" cm="1">
+        <f t="array" ref="B17">_xll.TICK(C17,D17)</f>
+        <v>Invalid request</v>
+      </c>
+      <c r="C17" t="s">
         <v>13</v>
       </c>
-      <c r="D13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>2775.5</v>
-      </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>0.95989999999999998</v>
-      </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" t="s">
-        <v>3</v>
+      <c r="D17" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Checks in sheet now working
</commit_message>
<xml_diff>
--- a/src/adaptors/xll/sheets/MarketData.xlsx
+++ b/src/adaptors/xll/sheets/MarketData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\trading\crypto\src\adaptors\xll\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E3232B-36E4-4A57-9D1C-959AD36449F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0D0018-6692-4A30-AD87-C523CA52325B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14895" yWindow="14715" windowWidth="28770" windowHeight="15570" xr2:uid="{6EC07C23-A19E-4BD9-8DD5-112772866BDB}"/>
+    <workbookView xWindow="14550" yWindow="14370" windowWidth="28770" windowHeight="15570" xr2:uid="{6EC07C23-A19E-4BD9-8DD5-112772866BDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -96,10 +96,10 @@
     <t>time</t>
   </si>
   <si>
-    <t>DUMMY</t>
-  </si>
-  <si>
     <t>ADABULL/USD</t>
+  </si>
+  <si>
+    <t>INVALID</t>
   </si>
 </sst>
 </file>
@@ -463,10 +463,13 @@
   <dimension ref="B2:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -482,7 +485,7 @@
         <v>OK</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -520,7 +523,7 @@
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" cm="1">
         <f t="array" ref="B8">_xll.TICK(C8,D8)</f>
-        <v>2249</v>
+        <v>2212.5</v>
       </c>
       <c r="D8" t="str">
         <f>$C$3</f>
@@ -530,7 +533,7 @@
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" cm="1">
         <f t="array" ref="B9">_xll.TICK(C9,D9)</f>
-        <v>2249</v>
+        <v>2212.5</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -543,7 +546,7 @@
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" cm="1">
         <f t="array" ref="B10">_xll.TICK(C10,D10)</f>
-        <v>2238</v>
+        <v>2201</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -553,16 +556,18 @@
         <v>ADABULL/USD</v>
       </c>
       <c r="E10">
-        <v>36282.5</v>
+        <f>SUM(B10:B11)/2</f>
+        <v>2212.5</v>
       </c>
       <c r="F10" t="b">
+        <f>E10=B9</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" cm="1">
         <f t="array" ref="B11">_xll.TICK(C11,D11)</f>
-        <v>2260</v>
+        <v>2224</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -575,7 +580,7 @@
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" cm="1">
         <f t="array" ref="B12">_xll.TICK(C12,D12)</f>
-        <v>2239</v>
+        <v>2204</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -588,7 +593,7 @@
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" cm="1">
         <f t="array" ref="B13">_xll.TICK(C13,D13)</f>
-        <v>1623128839.982069</v>
+        <v>1623132374.4572899</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -601,7 +606,7 @@
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" cm="1">
         <f t="array" ref="B14">_xll.TICK(C14,D14)</f>
-        <v>32937.5</v>
+        <v>32888</v>
       </c>
       <c r="D14" t="s">
         <v>2</v>
@@ -610,7 +615,7 @@
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" cm="1">
         <f t="array" ref="B15">_xll.TICK(C15,D15)</f>
-        <v>2505.5</v>
+        <v>2499.9</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
@@ -622,7 +627,7 @@
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" cm="1">
         <f t="array" ref="B16">_xll.TICK(C16,D16)</f>
-        <v>0.85882499999999995</v>
+        <v>0.85662499999999997</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
@@ -637,7 +642,7 @@
         <v>Invalid request</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D17" t="s">
         <v>2</v>

</xml_diff>